<commit_message>
* perf: :zap: Improve performance of binning fluence estimator
* test: :alembic: Add performance benchmark for FluenceEstimator::Binning.

* feat: :sparkles: Add a simple FluenceEstimator through binning

* refactor: :recycle: Move RaysHitMap and HitPoint to its own module.
</commit_message>
<xml_diff>
--- a/book/documents/FluenceSim.xlsx
+++ b/book/documents/FluenceSim.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ueisenb\AppData\Local\0_gsi_executables\opossum\book\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8602F7F7-A033-4574-9B61-1E3069E19AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D38F08-3DC9-4E30-A389-4F4856B08781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{31684BDE-C08B-4EE8-9776-19AE8F9583E1}"/>
+    <workbookView xWindow="1545" yWindow="0" windowWidth="20055" windowHeight="12195" xr2:uid="{31684BDE-C08B-4EE8-9776-19AE8F9583E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
   <si>
     <t>#of rays</t>
   </si>
@@ -53,6 +53,18 @@
   </si>
   <si>
     <t>theo</t>
+  </si>
+  <si>
+    <t>Binning</t>
+  </si>
+  <si>
+    <t>Binning method</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Sobol</t>
   </si>
 </sst>
 </file>
@@ -96,9 +108,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2663,6 +2678,189 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$E$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Binning</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$51:$A$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>241</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>301</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>367</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>439</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>517</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>613</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>721</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>823</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1459</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2263</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3259</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5815</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9060</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$E$51:$E$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>26900</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9261</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6594</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9289</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6150</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6142</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5455</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5089</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4209</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3661</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3033</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2625</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2233</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1954</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1092</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>702.40200000000004</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>486.98099999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>273.14600000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>242.715</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-588C-4F95-A14B-A5287A678C38}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2740,6 +2938,7 @@
         <c:axId val="1346431040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3724,6 +3923,633 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Binning</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$B$96</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>theory</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$97:$A$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$B$97:$B$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>159.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>159.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>159.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>159.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>159.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>159.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>159.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>159.19999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-617F-462B-A2B1-B1DEFAE81B3D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$C$96</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$97:$A$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$97:$C$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2476</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1161</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>759.31500000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>445.77499999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>370.34699999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>314.73399999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>306.923</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>211.39</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-617F-462B-A2B1-B1DEFAE81B3D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$D$96</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sobol</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$97:$A$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$D$97:$D$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3090</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1581</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>802.06200000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>398.358</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>240.90100000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>214.33199999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>190.69399999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>182.32300000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-617F-462B-A2B1-B1DEFAE81B3D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="254298784"/>
+        <c:axId val="254296704"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="254298784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="254296704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="254296704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="254298784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -4560,6 +5386,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6625,6 +7491,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7180,16 +8562,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>733424</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>247649</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7217,15 +8599,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7252,16 +8634,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>757236</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>623886</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>109536</xdr:rowOff>
+      <xdr:rowOff>90486</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>228599</xdr:colOff>
-      <xdr:row>92</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7281,6 +8663,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>595311</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Diagramm 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07B6BC55-CDDA-4091-8512-0ADD9091B689}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7627,18 +9045,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C703D84E-0E68-4C6B-AA21-624FA6B3E598}">
-  <dimension ref="A1:D92"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -8243,7 +9662,7 @@
         <v>157.41399999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
@@ -8256,8 +9675,11 @@
       <c r="D50" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E50" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>7</v>
       </c>
@@ -8270,8 +9692,11 @@
       <c r="D51">
         <v>64.507000000000005</v>
       </c>
+      <c r="E51">
+        <v>26900</v>
+      </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>19</v>
       </c>
@@ -8284,8 +9709,11 @@
       <c r="D52">
         <v>159.55000000000001</v>
       </c>
+      <c r="E52">
+        <v>10698</v>
+      </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>37</v>
       </c>
@@ -8298,8 +9726,11 @@
       <c r="D53">
         <v>194.75800000000001</v>
       </c>
+      <c r="E53">
+        <v>9261</v>
+      </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>61</v>
       </c>
@@ -8312,8 +9743,11 @@
       <c r="D54">
         <v>153.923</v>
       </c>
+      <c r="E54">
+        <v>6594</v>
+      </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>91</v>
       </c>
@@ -8326,8 +9760,11 @@
       <c r="D55">
         <v>263.21499999999997</v>
       </c>
+      <c r="E55">
+        <v>9289</v>
+      </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>127</v>
       </c>
@@ -8340,8 +9777,11 @@
       <c r="D56">
         <v>187.625</v>
       </c>
+      <c r="E56">
+        <v>6150</v>
+      </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>187</v>
       </c>
@@ -8354,8 +9794,11 @@
       <c r="D57">
         <v>317.72899999999998</v>
       </c>
+      <c r="E57">
+        <v>6142</v>
+      </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>241</v>
       </c>
@@ -8368,8 +9811,11 @@
       <c r="D58">
         <v>282.16300000000001</v>
       </c>
+      <c r="E58">
+        <v>5455</v>
+      </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>301</v>
       </c>
@@ -8382,8 +9828,11 @@
       <c r="D59">
         <v>492.34800000000001</v>
       </c>
+      <c r="E59">
+        <v>5089</v>
+      </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>367</v>
       </c>
@@ -8396,8 +9845,11 @@
       <c r="D60">
         <v>667.00099999999998</v>
       </c>
+      <c r="E60">
+        <v>4209</v>
+      </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>439</v>
       </c>
@@ -8410,8 +9862,11 @@
       <c r="D61">
         <v>634.80899999999997</v>
       </c>
+      <c r="E61">
+        <v>3661</v>
+      </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>517</v>
       </c>
@@ -8424,8 +9879,11 @@
       <c r="D62">
         <v>517.21299999999997</v>
       </c>
+      <c r="E62">
+        <v>3033</v>
+      </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>613</v>
       </c>
@@ -8438,8 +9896,11 @@
       <c r="D63">
         <v>477.27300000000002</v>
       </c>
+      <c r="E63">
+        <v>2625</v>
+      </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>721</v>
       </c>
@@ -8452,8 +9913,11 @@
       <c r="D64">
         <v>403.61500000000001</v>
       </c>
+      <c r="E64">
+        <v>2233</v>
+      </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>823</v>
       </c>
@@ -8466,8 +9930,11 @@
       <c r="D65">
         <v>609.22400000000005</v>
       </c>
+      <c r="E65">
+        <v>1954</v>
+      </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1459</v>
       </c>
@@ -8480,8 +9947,11 @@
       <c r="D66">
         <v>344.471</v>
       </c>
+      <c r="E66">
+        <v>1092</v>
+      </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2263</v>
       </c>
@@ -8494,8 +9964,11 @@
       <c r="D67">
         <v>309.66500000000002</v>
       </c>
+      <c r="E67">
+        <v>702.40200000000004</v>
+      </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>3259</v>
       </c>
@@ -8508,8 +9981,11 @@
       <c r="D68">
         <v>313.96199999999999</v>
       </c>
+      <c r="E68">
+        <v>486.98099999999999</v>
+      </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>5815</v>
       </c>
@@ -8522,8 +9998,11 @@
       <c r="D69">
         <v>267.12099999999998</v>
       </c>
+      <c r="E69">
+        <v>273.14600000000002</v>
+      </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>9060</v>
       </c>
@@ -8536,8 +10015,11 @@
       <c r="D70">
         <v>257.02600000000001</v>
       </c>
+      <c r="E70">
+        <v>242.715</v>
+      </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>0</v>
       </c>
@@ -8551,7 +10033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>7</v>
       </c>
@@ -8565,7 +10047,7 @@
         <v>67.668999999999997</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>19</v>
       </c>
@@ -8579,7 +10061,7 @@
         <v>46.374000000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>37</v>
       </c>
@@ -8593,7 +10075,7 @@
         <v>44.481999999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>61</v>
       </c>
@@ -8607,7 +10089,7 @@
         <v>78.536000000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>91</v>
       </c>
@@ -8621,7 +10103,7 @@
         <v>87.49</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>127</v>
       </c>
@@ -8635,7 +10117,7 @@
         <v>93.406999999999996</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>187</v>
       </c>
@@ -8649,7 +10131,7 @@
         <v>115.19799999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>241</v>
       </c>
@@ -8831,7 +10313,143 @@
         <v>301.66800000000001</v>
       </c>
     </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>500</v>
+      </c>
+      <c r="B97">
+        <v>159.19999999999999</v>
+      </c>
+      <c r="C97">
+        <v>2476</v>
+      </c>
+      <c r="D97">
+        <v>3090</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>1000</v>
+      </c>
+      <c r="B98">
+        <v>159.19999999999999</v>
+      </c>
+      <c r="C98">
+        <v>1161</v>
+      </c>
+      <c r="D98">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>2000</v>
+      </c>
+      <c r="B99">
+        <v>159.19999999999999</v>
+      </c>
+      <c r="C99">
+        <v>759.31500000000005</v>
+      </c>
+      <c r="D99">
+        <v>802.06200000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>4000</v>
+      </c>
+      <c r="B100">
+        <v>159.19999999999999</v>
+      </c>
+      <c r="C100">
+        <v>445.77499999999998</v>
+      </c>
+      <c r="D100">
+        <v>398.358</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>8000</v>
+      </c>
+      <c r="B101">
+        <v>159.19999999999999</v>
+      </c>
+      <c r="C101">
+        <v>370.34699999999998</v>
+      </c>
+      <c r="D101">
+        <v>240.90100000000001</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>16000</v>
+      </c>
+      <c r="B102">
+        <v>159.19999999999999</v>
+      </c>
+      <c r="C102">
+        <v>314.73399999999998</v>
+      </c>
+      <c r="D102">
+        <v>214.33199999999999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>32000</v>
+      </c>
+      <c r="B103">
+        <v>159.19999999999999</v>
+      </c>
+      <c r="C103">
+        <v>306.923</v>
+      </c>
+      <c r="D103">
+        <v>190.69399999999999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>64000</v>
+      </c>
+      <c r="B104">
+        <v>159.19999999999999</v>
+      </c>
+      <c r="C104">
+        <v>211.39</v>
+      </c>
+      <c r="D104">
+        <v>182.32300000000001</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A95:C95"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>